<commit_message>
Multiple fixes Prospective conso (renovation, destruction...)
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_ResTer_Heating_2D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_ResTer_Heating_2D.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="345" documentId="13_ncr:1_{84CDF3A1-E40C-9844-B681-EAA1EDD5B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FBE1F57-34A7-41F5-952D-2705719A2FD9}"/>
+  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{84CDF3A1-E40C-9844-B681-EAA1EDD5B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3A4AE4-5748-44A4-9A17-B0413B192B4F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
     <sheet name="retrofit_Transition" sheetId="2" r:id="rId2"/>
-    <sheet name="Energy_source" sheetId="11" r:id="rId3"/>
+    <sheet name="Energy_source_year" sheetId="11" r:id="rId3"/>
     <sheet name="Energy_source_Vecteur" sheetId="10" r:id="rId4"/>
     <sheet name="res_type_Energy_source" sheetId="4" r:id="rId5"/>
     <sheet name="EnergyS_buildingT_year" sheetId="13" r:id="rId6"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="48">
   <si>
     <t>Nom</t>
   </si>
@@ -148,28 +148,7 @@
     <t>peak_efficiency</t>
   </si>
   <si>
-    <t>init_conso_unitaire_elec</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_gaz</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_fioul</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_bois</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_charbon</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_ordures</t>
-  </si>
-  <si>
     <t>init_proportion_energy_need</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_autres</t>
   </si>
   <si>
     <t>autres</t>
@@ -188,6 +167,27 @@
   </si>
   <si>
     <t>old_taux_disp</t>
+  </si>
+  <si>
+    <t>conso_unitaire_elec</t>
+  </si>
+  <si>
+    <t>conso_unitaire_gaz</t>
+  </si>
+  <si>
+    <t>conso_unitaire_fioul</t>
+  </si>
+  <si>
+    <t>conso_unitaire_bois</t>
+  </si>
+  <si>
+    <t>conso_unitaire_charbon</t>
+  </si>
+  <si>
+    <t>conso_unitaire_ordures</t>
+  </si>
+  <si>
+    <t>conso_unitaire_autres</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +623,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>0.65283620689655175</v>
@@ -656,28 +656,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -685,42 +686,45 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.8</v>
+      <c r="C2" s="1">
+        <v>2020</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -729,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -740,16 +744,19 @@
       <c r="J2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
+      <c r="C3" s="1">
+        <v>2020</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -764,24 +771,27 @@
         <v>0</v>
       </c>
       <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
         <v>0.75</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
+      <c r="C4" s="1">
+        <v>2020</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -796,24 +806,27 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
         <v>0.75</v>
       </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
+      <c r="C5" s="1">
+        <v>2020</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -822,10 +835,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -836,16 +849,19 @@
       <c r="J5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
+      <c r="C6" s="1">
+        <v>2020</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -857,10 +873,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -868,16 +884,19 @@
       <c r="J6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2">
-        <v>0</v>
+      <c r="C7" s="1">
+        <v>2020</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -892,24 +911,27 @@
         <v>0</v>
       </c>
       <c r="H7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
+      <c r="C8" s="1">
+        <v>2020</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -921,27 +943,30 @@
         <v>0</v>
       </c>
       <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
         <v>0.75</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
       <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
         <v>0.25</v>
       </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
+      <c r="C9" s="1">
+        <v>2020</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -962,21 +987,24 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2">
-        <v>0.8</v>
+      <c r="C10" s="1">
+        <v>2020</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -985,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -996,16 +1024,19 @@
       <c r="J10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2">
-        <v>0</v>
+      <c r="C11" s="1">
+        <v>2020</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -1020,24 +1051,27 @@
         <v>0</v>
       </c>
       <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
         <v>0.75</v>
       </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2">
-        <v>0</v>
+      <c r="C12" s="1">
+        <v>2020</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -1052,24 +1086,27 @@
         <v>0</v>
       </c>
       <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
         <v>0.75</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
+      <c r="C13" s="1">
+        <v>2020</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -1078,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -1092,16 +1129,19 @@
       <c r="J13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2">
-        <v>0</v>
+      <c r="C14" s="1">
+        <v>2020</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -1113,10 +1153,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -1124,16 +1164,19 @@
       <c r="J14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2">
-        <v>0</v>
+      <c r="C15" s="1">
+        <v>2020</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1148,24 +1191,27 @@
         <v>0</v>
       </c>
       <c r="H15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="2">
-        <v>0</v>
+      <c r="C16" s="1">
+        <v>2020</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -1177,27 +1223,30 @@
         <v>0</v>
       </c>
       <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
         <v>0.75</v>
       </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
       <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
         <v>0.25</v>
       </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2">
-        <v>0</v>
+      <c r="C17" s="1">
+        <v>2020</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -1218,21 +1267,24 @@
         <v>0</v>
       </c>
       <c r="J17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2">
-        <v>0.8</v>
+      <c r="C18" s="1">
+        <v>2020</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1241,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -1252,16 +1304,19 @@
       <c r="J18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="2">
-        <v>0</v>
+      <c r="C19" s="1">
+        <v>2020</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -1276,24 +1331,27 @@
         <v>0</v>
       </c>
       <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
         <v>0.75</v>
       </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2">
-        <v>0</v>
+      <c r="C20" s="1">
+        <v>2020</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -1308,24 +1366,27 @@
         <v>0</v>
       </c>
       <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
         <v>0.75</v>
       </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2">
-        <v>0</v>
+      <c r="C21" s="1">
+        <v>2020</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -1334,10 +1395,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -1348,16 +1409,19 @@
       <c r="J21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2">
-        <v>0</v>
+      <c r="C22" s="1">
+        <v>2020</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -1369,10 +1433,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -1380,16 +1444,19 @@
       <c r="J22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2">
-        <v>0</v>
+      <c r="C23" s="1">
+        <v>2020</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -1404,24 +1471,27 @@
         <v>0</v>
       </c>
       <c r="H23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>0</v>
+      <c r="C24" s="1">
+        <v>2020</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
@@ -1433,27 +1503,30 @@
         <v>0</v>
       </c>
       <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
         <v>0.75</v>
       </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
       <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
         <v>0.25</v>
       </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2">
-        <v>0</v>
+      <c r="C25" s="1">
+        <v>2020</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -1474,6 +1547,849 @@
         <v>0</v>
       </c>
       <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>1</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1488,7 +2404,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1507,25 +2423,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1629,20 +2545,20 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="E5" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>0.23799999999999999</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="G5" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="H5" s="2">
-        <v>0.248</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="I5" s="2">
         <f>1-SUM(C5:H5)</f>
-        <v>0.12</v>
+        <v>0.10699999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2028,7 +2944,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2172,7 +3088,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2">
         <v>0.85</v>
@@ -2280,7 +3196,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2309,7 +3225,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2807,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5AE5BC-45EB-447C-8E62-14DCFBF41CB2}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2827,7 +3743,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2869,7 +3785,7 @@
         <v>2020</v>
       </c>
       <c r="D4" s="2">
-        <v>3000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2911,7 +3827,7 @@
         <v>2020</v>
       </c>
       <c r="D7" s="2">
-        <v>2400000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2925,7 +3841,7 @@
         <v>2020</v>
       </c>
       <c r="D8" s="2">
-        <v>1200000</v>
+        <v>2400000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2939,7 +3855,7 @@
         <v>2020</v>
       </c>
       <c r="D9" s="2">
-        <v>600000</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3093,7 +4009,7 @@
         <v>2020</v>
       </c>
       <c r="D20" s="2">
-        <v>2625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -3135,7 +4051,7 @@
         <v>2020</v>
       </c>
       <c r="D23" s="2">
-        <v>2625000</v>
+        <v>1750000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -3149,7 +4065,7 @@
         <v>2020</v>
       </c>
       <c r="D24" s="2">
-        <v>4375000</v>
+        <v>6125000</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -3163,7 +4079,7 @@
         <v>2020</v>
       </c>
       <c r="D25" s="2">
-        <v>2625000</v>
+        <v>4375000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3317,7 +4233,7 @@
         <v>2020</v>
       </c>
       <c r="D36" s="2">
-        <v>1875000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -3359,7 +4275,7 @@
         <v>2020</v>
       </c>
       <c r="D39" s="2">
-        <v>1500000</v>
+        <v>1875000</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3373,7 +4289,7 @@
         <v>2020</v>
       </c>
       <c r="D40" s="2">
-        <v>750000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -3387,7 +4303,7 @@
         <v>2020</v>
       </c>
       <c r="D41" s="2">
-        <v>375000</v>
+        <v>1125000</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -3516,8 +4432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D0F366-6237-48BA-A474-DA6D4716EB8C}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3623,13 +4539,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B8" s="5">
         <v>2020</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3646,7 +4562,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>79</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3721,13 +4637,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5">
         <v>2050</v>
       </c>
       <c r="C15" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3744,7 +4660,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3853,10 +4769,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Multiple fixes Prospective conso (renovation, destruction, construction etc...)
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_ResTer_Heating_2D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_ResTer_Heating_2D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{84CDF3A1-E40C-9844-B681-EAA1EDD5B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3A4AE4-5748-44A4-9A17-B0413B192B4F}"/>
+  <xr:revisionPtr revIDLastSave="446" documentId="13_ncr:1_{84CDF3A1-E40C-9844-B681-EAA1EDD5B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92FFD80D-225A-457B-A8BF-74D4279D6465}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="47">
   <si>
     <t>Nom</t>
   </si>
@@ -154,9 +154,6 @@
     <t>autres</t>
   </si>
   <si>
-    <t>biogas_share</t>
-  </si>
-  <si>
     <t>share_peak</t>
   </si>
   <si>
@@ -239,7 +236,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -273,11 +270,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -299,6 +305,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2404,7 +2413,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2423,25 +2432,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2944,7 +2953,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3193,10 +3202,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3208,7 +3217,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3225,10 +3234,12 @@
         <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3248,7 +3259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3268,7 +3279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3288,7 +3299,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3299,7 +3310,7 @@
         <v>3995209</v>
       </c>
       <c r="D5" s="2">
-        <v>167.49279128952941</v>
+        <v>72.82295273457801</v>
       </c>
       <c r="E5" s="2">
         <v>52.973740041026069</v>
@@ -3308,7 +3319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3328,7 +3339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3339,7 +3350,7 @@
         <v>636489.75</v>
       </c>
       <c r="D7" s="2">
-        <v>147.12858456177321</v>
+        <v>63.968949809466615</v>
       </c>
       <c r="E7" s="2">
         <v>44.438915275434461</v>
@@ -3348,7 +3359,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -3359,7 +3370,7 @@
         <v>146882.25</v>
       </c>
       <c r="D8" s="2">
-        <v>33.952750283486118</v>
+        <v>14.762065340646139</v>
       </c>
       <c r="E8" s="2">
         <v>10.255134294331031</v>
@@ -3368,7 +3379,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -3379,7 +3390,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>33.952750283486118</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -3388,7 +3399,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3408,7 +3419,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -3428,7 +3439,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3470,7 @@
         <v>4442744</v>
       </c>
       <c r="D13" s="2">
-        <v>186.3295070204899</v>
+        <v>81.012829139343438</v>
       </c>
       <c r="E13" s="2">
         <v>105.71703104202599</v>
@@ -3468,7 +3479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -3488,7 +3499,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3499,7 +3510,7 @@
         <v>365907.75</v>
       </c>
       <c r="D15" s="2">
-        <v>146.6052858044018</v>
+        <v>63.741428610609482</v>
       </c>
       <c r="E15" s="2">
         <v>92.499838314799049</v>
@@ -3508,7 +3519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3519,7 +3530,7 @@
         <v>84440.25</v>
       </c>
       <c r="D16" s="2">
-        <v>33.831989031785021</v>
+        <v>14.709560448602184</v>
       </c>
       <c r="E16" s="2">
         <v>21.3461165341844</v>
@@ -3539,7 +3550,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>33.831989031785021</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -3619,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>219.82137857142857</v>
+        <v>95.574512422360257</v>
       </c>
       <c r="E21" s="2">
         <v>204120000</v>
@@ -3659,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>210.89125000000001</v>
+        <v>91.69184782608697</v>
       </c>
       <c r="E23" s="2">
         <v>13996800</v>
@@ -3679,7 +3690,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>221.04354189336235</v>
+        <v>96.105887779722764</v>
       </c>
       <c r="E24" s="2">
         <v>89326800</v>
@@ -3699,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="2">
-        <v>221.04354189336235</v>
+        <v>0</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
@@ -3723,7 +3734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5AE5BC-45EB-447C-8E62-14DCFBF41CB2}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3743,7 +3754,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4750,10 +4761,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E4D7B8-7F8A-6D47-8E14-1AE459D21508}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4761,7 +4772,7 @@
     <col min="1" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -4769,13 +4780,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>2020</v>
       </c>
@@ -4783,85 +4791,76 @@
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2022</v>
       </c>
       <c r="B3" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8">
+      <c r="C3" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2025</v>
       </c>
       <c r="B4" s="7">
         <v>0.10000000000000002</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8">
+      <c r="C4" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2030</v>
       </c>
       <c r="B5" s="7">
         <v>0.34999999999999992</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8">
+      <c r="C5" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2035</v>
       </c>
       <c r="B6" s="7">
         <v>0.69999999999999984</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8">
+      <c r="C6" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2040</v>
       </c>
       <c r="B7" s="7">
         <v>0.85</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8">
+      <c r="C7" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>2045</v>
       </c>
       <c r="B8" s="7">
         <v>0.94999999999999984</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8">
+      <c r="C8" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>2050</v>
       </c>
@@ -4869,9 +4868,6 @@
         <v>1</v>
       </c>
       <c r="C9" s="8">
-        <v>0</v>
-      </c>
-      <c r="D9" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>

</xml_diff>